<commit_message>
0.0.15: Add generateToJson flag as ant task input
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectTsTask.xlsx
+++ b/meta/program/BlancoValueObjectTsTask.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2985AE-FCEF-5841-9890-DA3D4F7EDEB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225E21F7-2D0B-6D4D-AB30-0C56A0D4F487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -362,6 +362,17 @@
   </si>
   <si>
     <t>lineSeparator</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>generateToJson</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>toJSONメソッドを生成します</t>
+    <rPh sb="11" eb="13">
+      <t xml:space="preserve">セイセイ </t>
+    </rPh>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -1357,10 +1368,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23:I23"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1560,7 +1571,7 @@
     </row>
     <row r="16" spans="1:9" ht="27" customHeight="1">
       <c r="A16" s="49">
-        <f t="shared" ref="A16:A23" si="0">A15+1</f>
+        <f t="shared" ref="A16:A24" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="50" t="s">
@@ -1730,16 +1741,27 @@
       <c r="H23" s="64"/>
       <c r="I23" s="65"/>
     </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="42"/>
+    <row r="24" spans="1:9" ht="52" customHeight="1">
+      <c r="A24" s="49">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>21</v>
+      </c>
       <c r="D24" s="24"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="27"/>
+      <c r="E24" s="61" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="65"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="22"/>
@@ -1775,18 +1797,31 @@
       <c r="I27" s="27"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="28"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="33"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="27"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="F12:I13"/>
+    <mergeCell ref="F24:I24"/>
     <mergeCell ref="F23:I23"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
@@ -1802,18 +1837,17 @@
     <mergeCell ref="F21:I21"/>
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F12:I13"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F44" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F45" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D28" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D29" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>必須</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C28" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C29" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>型リスト</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
0.0.17: searchTmpdir option is available, for creating listClass.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectTsTask.xlsx
+++ b/meta/program/BlancoValueObjectTsTask.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225E21F7-2D0B-6D4D-AB30-0C56A0D4F487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3BCF3E-1AD2-CB4B-9459-1846A925C010}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -375,12 +375,38 @@
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
+  <si>
+    <t>searchTmpdir</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>listClassの対象とするtmpディレクトリをカンマ区切りで指定します。指定ディレクトリ直下のvalueobjectディレクトリの下にxmlを探しにいきます。</t>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">タイショウトスル </t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t xml:space="preserve">チョッカ </t>
+    </rPh>
+    <rPh sb="67" eb="68">
+      <t xml:space="preserve">シタニ </t>
+    </rPh>
+    <rPh sb="73" eb="74">
+      <t xml:space="preserve">サガシニ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -433,6 +459,12 @@
       <family val="2"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -840,7 +872,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -946,6 +978,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -994,12 +1032,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1371,7 +1411,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F25" sqref="F25:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1417,10 +1457,10 @@
       <c r="F5"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="66"/>
+      <c r="B6" s="68"/>
       <c r="C6" s="6" t="s">
         <v>43</v>
       </c>
@@ -1430,10 +1470,10 @@
       <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="66"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="6" t="s">
         <v>44</v>
       </c>
@@ -1444,10 +1484,10 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="66"/>
+      <c r="B8" s="68"/>
       <c r="C8" s="6" t="s">
         <v>45</v>
       </c>
@@ -1458,10 +1498,10 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="66"/>
+      <c r="B9" s="68"/>
       <c r="C9" s="11" t="s">
         <v>7</v>
       </c>
@@ -1493,38 +1533,38 @@
       <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="13.5" customHeight="1">
-      <c r="A12" s="70" t="s">
+      <c r="A12" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="71" t="s">
+      <c r="C12" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="72" t="s">
+      <c r="D12" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="73" t="s">
+      <c r="E12" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="81" t="s">
+      <c r="F12" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="82"/>
-      <c r="H12" s="82"/>
-      <c r="I12" s="82"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="70"/>
-      <c r="B13" s="70"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="82"/>
+      <c r="A13" s="72"/>
+      <c r="B13" s="72"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
     </row>
     <row r="14" spans="1:9" ht="27" customHeight="1">
       <c r="A14" s="44">
@@ -1540,12 +1580,12 @@
         <v>13</v>
       </c>
       <c r="E14" s="48"/>
-      <c r="F14" s="67" t="s">
+      <c r="F14" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="69"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="71"/>
     </row>
     <row r="15" spans="1:9" ht="27" customHeight="1">
       <c r="A15" s="49">
@@ -1562,16 +1602,16 @@
       <c r="E15" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="77" t="s">
+      <c r="F15" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="79"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="81"/>
     </row>
     <row r="16" spans="1:9" ht="27" customHeight="1">
       <c r="A16" s="49">
-        <f t="shared" ref="A16:A24" si="0">A15+1</f>
+        <f t="shared" ref="A16:A25" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="50" t="s">
@@ -1584,12 +1624,12 @@
       <c r="E16" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="80" t="s">
+      <c r="F16" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="79"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="81"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="49">
@@ -1692,12 +1732,12 @@
       <c r="E21" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="74" t="s">
+      <c r="F21" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="75"/>
-      <c r="H21" s="75"/>
-      <c r="I21" s="76"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77"/>
+      <c r="I21" s="78"/>
     </row>
     <row r="22" spans="1:9" ht="52" customHeight="1">
       <c r="A22" s="49">
@@ -1712,12 +1752,12 @@
       </c>
       <c r="D22" s="24"/>
       <c r="E22" s="25"/>
-      <c r="F22" s="63" t="s">
+      <c r="F22" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="65"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="67"/>
     </row>
     <row r="23" spans="1:9" ht="52" customHeight="1">
       <c r="A23" s="49">
@@ -1734,12 +1774,12 @@
       <c r="E23" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="F23" s="63" t="s">
+      <c r="F23" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="65"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="67"/>
     </row>
     <row r="24" spans="1:9" ht="52" customHeight="1">
       <c r="A24" s="49">
@@ -1756,23 +1796,32 @@
       <c r="E24" s="61" t="b">
         <v>0</v>
       </c>
-      <c r="F24" s="63" t="s">
+      <c r="F24" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="G24" s="64"/>
-      <c r="H24" s="64"/>
-      <c r="I24" s="65"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="67"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="22"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="27"/>
+      <c r="A25" s="83">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B25" s="84" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="85"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="66"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="67"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="22"/>
@@ -1819,7 +1868,9 @@
       <c r="I29" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="18">
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F25:I25"/>
     <mergeCell ref="F12:I13"/>
     <mergeCell ref="F24:I24"/>
     <mergeCell ref="F23:I23"/>
@@ -1836,7 +1887,6 @@
     <mergeCell ref="F22:I22"/>
     <mergeCell ref="F21:I21"/>
     <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="3">
@@ -1844,10 +1894,10 @@
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D29" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D24 D26:D29" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>必須</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C29" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C24 C26:C29" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>型リスト</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>